<commit_message>
New music for cutscenes
Added Audio Bank 4 for cutscene music
Load Audio Bank 4 in cutprincess fn
Need to load game audio bank back in afterwards
Bug with sfx disappearing until after playing music (vgm player init) is
back
Need sfx state machine
</commit_message>
<xml_diff>
--- a/Notes/music.xlsx
+++ b/Notes/music.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kconnell\OneDrive\BEEB\Repos\pop-beeb\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{162A5275-00C3-4FE0-8FA3-DFD4B6C81E65}"/>
+  <xr:revisionPtr revIDLastSave="339" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{EE430423-3704-462A-B7DE-645929AAC9BB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3218" windowHeight="1605" xr2:uid="{19CB3A3B-005F-4A7A-B3B3-7B2FCB2886A0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="107">
   <si>
     <t>Game music</t>
   </si>
@@ -343,6 +343,15 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>m-cutscene-pre2_4_6_C.</t>
+  </si>
+  <si>
+    <t>m-cutscene-notmuchtime</t>
+  </si>
+  <si>
+    <t>m-cutscene-pre8_9</t>
   </si>
 </sst>
 </file>
@@ -366,12 +375,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -386,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,6 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864DF1D0-1AEF-4269-82FC-BFE1E4A43248}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -833,7 +849,7 @@
       <c r="G4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="5" t="s">
         <v>46</v>
       </c>
       <c r="I4" s="1">
@@ -938,7 +954,7 @@
       <c r="G7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="5" t="s">
         <v>47</v>
       </c>
       <c r="I7" s="1">
@@ -967,7 +983,7 @@
       <c r="G8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="5" t="s">
         <v>47</v>
       </c>
       <c r="I8" s="1">
@@ -1002,14 +1018,14 @@
       <c r="G9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="5" t="s">
         <v>48</v>
       </c>
       <c r="I9" s="1">
         <v>3</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1034,7 +1050,7 @@
       <c r="F10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="5" t="s">
         <v>48</v>
       </c>
       <c r="I10" s="1">
@@ -1060,7 +1076,7 @@
       <c r="F11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="5" t="s">
         <v>48</v>
       </c>
       <c r="I11" s="1">
@@ -1089,7 +1105,7 @@
       <c r="G12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="5" t="s">
         <v>47</v>
       </c>
       <c r="I12" s="1">
@@ -1153,7 +1169,7 @@
       <c r="G14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="I14" s="1">
@@ -1171,7 +1187,7 @@
       <c r="G16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1187,8 +1203,20 @@
       <c r="E17" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3</v>
+      </c>
+      <c r="J17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1213,8 +1241,11 @@
       <c r="I18" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1239,8 +1270,11 @@
       <c r="I19" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1259,14 +1293,17 @@
       <c r="G20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="5" t="s">
         <v>46</v>
       </c>
       <c r="I20" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1285,14 +1322,14 @@
       <c r="G21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="5" t="s">
         <v>47</v>
       </c>
       <c r="I21" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1311,8 +1348,11 @@
       <c r="G22" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1337,8 +1377,11 @@
       <c r="I23" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>101</v>
       </c>
@@ -1355,7 +1398,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
@@ -1366,7 +1409,7 @@
       <c r="G26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1380,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1388,7 +1431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1402,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1416,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Added small potion ditty
For when player drinks recharge potion
</commit_message>
<xml_diff>
--- a/Notes/music.xlsx
+++ b/Notes/music.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kconnell\OneDrive\BEEB\Repos\pop-beeb\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{EE430423-3704-462A-B7DE-645929AAC9BB}"/>
+  <xr:revisionPtr revIDLastSave="408" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{ADEF8C23-4FAD-41CA-A8F8-5B1E148128BE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3218" windowHeight="1605" xr2:uid="{19CB3A3B-005F-4A7A-B3B3-7B2FCB2886A0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="113">
   <si>
     <t>Game music</t>
   </si>
@@ -39,9 +39,6 @@
     <t>accidental death</t>
   </si>
   <si>
-    <t>danger theme for mirror (level 4)</t>
-  </si>
-  <si>
     <t>got sword</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>s_Curtain</t>
   </si>
   <si>
-    <t>Current mapping</t>
-  </si>
-  <si>
     <t>pop_music_death</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
     <t>should do</t>
   </si>
   <si>
-    <t>Best match</t>
-  </si>
-  <si>
     <t>Prince of Persia - 07 - Death</t>
   </si>
   <si>
@@ -297,9 +288,6 @@
     <t>Princess standing</t>
   </si>
   <si>
-    <t>1, 4, 6 (cut5=pre12)</t>
-  </si>
-  <si>
     <t>m-begin</t>
   </si>
   <si>
@@ -336,29 +324,59 @@
     <t>Cut3 = pre6</t>
   </si>
   <si>
-    <t>&lt;none&gt;</t>
-  </si>
-  <si>
     <t>Ominous (time running out) (or Cut1)</t>
   </si>
   <si>
     <t>?</t>
   </si>
   <si>
-    <t>m-cutscene-pre2_4_6_C.</t>
-  </si>
-  <si>
     <t>m-cutscene-notmuchtime</t>
   </si>
   <si>
     <t>m-cutscene-pre8_9</t>
+  </si>
+  <si>
+    <t>1, 4, 6</t>
+  </si>
+  <si>
+    <t>danger theme for entrance (level 1), mirror (level 4)</t>
+  </si>
+  <si>
+    <t>cutscene_not_much_time_left</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>m-cutscene-pre2_4_6_C</t>
+  </si>
+  <si>
+    <t>Code label</t>
+  </si>
+  <si>
+    <t>pop_music_tragic</t>
+  </si>
+  <si>
+    <t>pop_music_timer</t>
+  </si>
+  <si>
+    <t>pop_music_heartbeat</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>pop_music_lifepotion</t>
+  </si>
+  <si>
+    <t>m-potion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,8 +392,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,6 +413,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -398,10 +428,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,8 +443,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,21 +763,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864DF1D0-1AEF-4269-82FC-BFE1E4A43248}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15.86328125" customWidth="1"/>
     <col min="2" max="2" width="9.06640625" style="1"/>
-    <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.9296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.86328125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.796875" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.06640625" style="1"/>
+    <col min="7" max="7" width="39.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -759,42 +794,42 @@
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -803,159 +838,144 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I3" s="1">
         <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3">
-        <v>365</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I4" s="1">
         <v>3</v>
       </c>
-      <c r="J4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I5" s="1">
         <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>89</v>
-      </c>
-      <c r="K5">
-        <v>267</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I6" s="1">
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>91</v>
-      </c>
-      <c r="K6">
-        <v>370</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" s="1">
         <v>3</v>
@@ -963,95 +983,86 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I8" s="1">
         <v>3</v>
       </c>
-      <c r="J8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>48</v>
+        <v>68</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
       </c>
       <c r="I9" s="1">
         <v>3</v>
       </c>
-      <c r="J9" t="s">
-        <v>91</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I10" s="1">
         <v>3</v>
@@ -1059,25 +1070,28 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>63</v>
+      <c r="G11" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I11" s="1">
         <v>3</v>
@@ -1085,28 +1099,28 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1">
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12" s="1">
         <v>3</v>
@@ -1114,71 +1128,71 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="I13" s="1">
         <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>90</v>
-      </c>
-      <c r="K13">
-        <v>385</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1">
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>49</v>
+        <v>70</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
       </c>
       <c r="I14" s="1">
         <v>3</v>
       </c>
+      <c r="J14" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B16" s="4"/>
       <c r="D16" s="4"/>
@@ -1189,218 +1203,224 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="H17" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="I17" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="I18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="I19" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1">
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>46</v>
+        <v>77</v>
+      </c>
+      <c r="H20" t="s">
+        <v>107</v>
       </c>
       <c r="I20" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1">
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I21" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="H22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I22" s="1">
+        <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1">
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="I23" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J23" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="4"/>
       <c r="D26" s="4"/>
@@ -1411,13 +1431,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -1425,7 +1445,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1">
         <v>2</v>
@@ -1433,13 +1453,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1">
         <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I29" s="1">
         <v>0</v>
@@ -1447,13 +1467,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1">
         <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I30" s="1">
         <v>1</v>
@@ -1461,7 +1481,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1">
         <v>5</v>
@@ -1469,13 +1489,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1">
         <v>7</v>
       </c>
       <c r="H33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I33" s="1">
         <v>1</v>
@@ -1483,7 +1503,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1">
         <v>8</v>
@@ -1491,7 +1511,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1">
         <v>9</v>
@@ -1499,7 +1519,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" s="1">
         <v>10</v>
@@ -1507,7 +1527,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="1">
         <v>11</v>
@@ -1515,7 +1535,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1">
         <v>12</v>
@@ -1523,7 +1543,7 @@
     </row>
     <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="4"/>
       <c r="D40" s="4"/>
@@ -1534,7 +1554,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -1542,7 +1562,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
Using pucrunch to shrink all MODE 2 screens for the attract sequence
pu.bat batch file to compress all mode2.bin screens with correct params
Brought over unpack.asm from retrosoftware pucrunch wiki page
Some tweaks to master.asm to make things work
Main thing is not quite having in-place decompress so need one page
extra
This only works because the last line of all the MODE 2 screens is
blank!
But does mean we can fit all the attract sequence files on side A of the
disc
</commit_message>
<xml_diff>
--- a/Notes/music.xlsx
+++ b/Notes/music.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kconnell\OneDrive\BEEB\Repos\pop-beeb\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="408" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{ADEF8C23-4FAD-41CA-A8F8-5B1E148128BE}"/>
+  <xr:revisionPtr revIDLastSave="414" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{1CD3FDBB-7E6F-47FF-8B6A-9876496C76A3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3218" windowHeight="1605" xr2:uid="{19CB3A3B-005F-4A7A-B3B3-7B2FCB2886A0}"/>
   </bookViews>
@@ -327,9 +327,6 @@
     <t>Ominous (time running out) (or Cut1)</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>m-cutscene-notmuchtime</t>
   </si>
   <si>
@@ -370,6 +367,9 @@
   </si>
   <si>
     <t>m-potion</t>
+  </si>
+  <si>
+    <t>tbd</t>
   </si>
 </sst>
 </file>
@@ -764,7 +764,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -815,13 +815,13 @@
         <v>64</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>51</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>63</v>
@@ -896,13 +896,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>60</v>
@@ -934,7 +934,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>60</v>
@@ -966,7 +966,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>60</v>
@@ -995,7 +995,7 @@
         <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>59</v>
@@ -1059,7 +1059,7 @@
         <v>60</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>46</v>
@@ -1111,7 +1111,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>60</v>
@@ -1149,7 +1149,7 @@
         <v>69</v>
       </c>
       <c r="H13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I13" s="1">
         <v>3</v>
@@ -1172,7 +1172,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>54</v>
@@ -1187,7 +1187,7 @@
         <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -1218,16 +1218,16 @@
         <v>54</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I17" s="1">
         <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
@@ -1250,13 +1250,13 @@
         <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I18" s="1">
         <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
@@ -1279,13 +1279,13 @@
         <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I19" s="1">
         <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
@@ -1308,13 +1308,13 @@
         <v>77</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I20" s="1">
         <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
@@ -1363,13 +1363,13 @@
         <v>74</v>
       </c>
       <c r="H22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I22" s="1">
         <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
@@ -1392,18 +1392,18 @@
         <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I23" s="1">
         <v>4</v>
       </c>
       <c r="J23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Updated lifepotion to work with glug
</commit_message>
<xml_diff>
--- a/Notes/music.xlsx
+++ b/Notes/music.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kconnell\OneDrive\BEEB\Repos\pop-beeb\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="414" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{1CD3FDBB-7E6F-47FF-8B6A-9876496C76A3}"/>
+  <xr:revisionPtr revIDLastSave="430" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{AE73A80D-13F5-4CC7-838B-CDB150F435A3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3218" windowHeight="1605" xr2:uid="{19CB3A3B-005F-4A7A-B3B3-7B2FCB2886A0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
   <si>
     <t>Game music</t>
   </si>
@@ -219,9 +219,6 @@
     <t>should do</t>
   </si>
   <si>
-    <t>Prince of Persia - 07 - Death</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -370,6 +367,21 @@
   </si>
   <si>
     <t>tbd</t>
+  </si>
+  <si>
+    <t>pop_music_heroic</t>
+  </si>
+  <si>
+    <t>pop_music_rejoin</t>
+  </si>
+  <si>
+    <t>m-playerdeath-reg</t>
+  </si>
+  <si>
+    <t>m-playerdeath-sword</t>
+  </si>
+  <si>
+    <t>m-story5-end-merge-bla</t>
   </si>
 </sst>
 </file>
@@ -764,7 +776,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -806,25 +818,25 @@
         <v>52</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>58</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>51</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
@@ -847,7 +859,7 @@
         <v>59</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3" t="s">
         <v>44</v>
@@ -856,7 +868,7 @@
         <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
@@ -879,13 +891,16 @@
         <v>59</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>44</v>
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
+        <v>112</v>
       </c>
       <c r="I4" s="1">
         <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -896,19 +911,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H5" t="s">
         <v>45</v>
@@ -917,7 +932,7 @@
         <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
@@ -934,22 +949,22 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>46</v>
       </c>
       <c r="I6" s="1">
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
@@ -966,19 +981,22 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>46</v>
+        <v>70</v>
+      </c>
+      <c r="H7" t="s">
+        <v>113</v>
       </c>
       <c r="I7" s="1">
         <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
@@ -995,13 +1013,13 @@
         <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>44</v>
@@ -1030,7 +1048,7 @@
         <v>54</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s">
         <v>46</v>
@@ -1059,7 +1077,7 @@
         <v>60</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>46</v>
@@ -1088,13 +1106,16 @@
         <v>61</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>46</v>
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
+        <v>113</v>
       </c>
       <c r="I11" s="1">
         <v>3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
@@ -1111,13 +1132,13 @@
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>45</v>
@@ -1146,16 +1167,16 @@
         <v>54</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I13" s="1">
         <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
@@ -1172,13 +1193,13 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
         <v>47</v>
@@ -1187,12 +1208,12 @@
         <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="4"/>
       <c r="D16" s="4"/>
@@ -1209,25 +1230,25 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I17" s="1">
         <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
@@ -1238,25 +1259,25 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I18" s="1">
         <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
@@ -1267,25 +1288,25 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I19" s="1">
         <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
@@ -1296,25 +1317,25 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I20" s="1">
         <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
@@ -1325,16 +1346,16 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>45</v>
@@ -1351,25 +1372,25 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I22" s="1">
         <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
@@ -1380,42 +1401,42 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I23" s="1">
         <v>4</v>
       </c>
       <c r="J23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Added new in-game tunes
Killed by Shadow
Meet Jaffar
</commit_message>
<xml_diff>
--- a/Notes/music.xlsx
+++ b/Notes/music.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kconnell\OneDrive\BEEB\Repos\pop-beeb\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="430" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{AE73A80D-13F5-4CC7-838B-CDB150F435A3}"/>
+  <xr:revisionPtr revIDLastSave="444" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{91BD5E2F-22B9-41B3-92FF-9F919304701F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3218" windowHeight="1605" xr2:uid="{19CB3A3B-005F-4A7A-B3B3-7B2FCB2886A0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="121">
   <si>
     <t>Game music</t>
   </si>
@@ -291,9 +291,6 @@
     <t>m-lifepotion</t>
   </si>
   <si>
-    <t>Prince of Persia - 05 - Get Sword</t>
-  </si>
-  <si>
     <t>Cut8 = pre8</t>
   </si>
   <si>
@@ -382,13 +379,28 @@
   </si>
   <si>
     <t>m-story5-end-merge-bla</t>
+  </si>
+  <si>
+    <t>pop_music_shadow</t>
+  </si>
+  <si>
+    <t>pop_music_jaffar</t>
+  </si>
+  <si>
+    <t>m_jaffar</t>
+  </si>
+  <si>
+    <t>m-e4-killedbyshadow</t>
+  </si>
+  <si>
+    <t>m-killguard-or-sword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,15 +416,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,11 +430,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -440,9 +440,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -455,12 +454,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -775,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864DF1D0-1AEF-4269-82FC-BFE1E4A43248}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -818,7 +816,7 @@
         <v>52</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>58</v>
@@ -827,13 +825,13 @@
         <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>51</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>62</v>
@@ -868,7 +866,7 @@
         <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
@@ -894,13 +892,13 @@
         <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I4" s="1">
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -911,18 +909,18 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="1" t="s">
         <v>71</v>
       </c>
       <c r="H5" t="s">
@@ -949,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>60</v>
@@ -957,14 +955,14 @@
       <c r="G6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" t="s">
         <v>46</v>
       </c>
       <c r="I6" s="1">
         <v>3</v>
       </c>
-      <c r="J6" t="s">
-        <v>86</v>
+      <c r="J6" s="6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
@@ -981,7 +979,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>60</v>
@@ -990,13 +988,13 @@
         <v>70</v>
       </c>
       <c r="H7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I7" s="1">
         <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
@@ -1013,7 +1011,7 @@
         <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>59</v>
@@ -1021,11 +1019,14 @@
       <c r="G8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>44</v>
+      <c r="H8" t="s">
+        <v>116</v>
       </c>
       <c r="I8" s="1">
         <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
@@ -1056,6 +1057,9 @@
       <c r="I9" s="1">
         <v>3</v>
       </c>
+      <c r="J9" s="6" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -1077,11 +1081,9 @@
         <v>60</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>46</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="1">
         <v>3</v>
       </c>
@@ -1109,13 +1111,13 @@
         <v>70</v>
       </c>
       <c r="H11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I11" s="1">
         <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
@@ -1132,7 +1134,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>60</v>
@@ -1141,10 +1143,13 @@
         <v>75</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="I12" s="1">
         <v>3</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
@@ -1170,7 +1175,7 @@
         <v>68</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I13" s="1">
         <v>3</v>
@@ -1193,7 +1198,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>54</v>
@@ -1208,7 +1213,7 @@
         <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -1230,25 +1235,25 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I17" s="1">
         <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
@@ -1262,7 +1267,7 @@
         <v>83</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>54</v>
@@ -1271,13 +1276,13 @@
         <v>73</v>
       </c>
       <c r="H18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I18" s="1">
         <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
@@ -1291,7 +1296,7 @@
         <v>83</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>54</v>
@@ -1300,13 +1305,13 @@
         <v>73</v>
       </c>
       <c r="H19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I19" s="1">
         <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
@@ -1320,7 +1325,7 @@
         <v>81</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>54</v>
@@ -1329,13 +1334,13 @@
         <v>76</v>
       </c>
       <c r="H20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I20" s="1">
         <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
@@ -1349,7 +1354,7 @@
         <v>80</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>54</v>
@@ -1375,7 +1380,7 @@
         <v>82</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>54</v>
@@ -1384,13 +1389,13 @@
         <v>73</v>
       </c>
       <c r="H22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I22" s="1">
         <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
@@ -1404,7 +1409,7 @@
         <v>78</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>54</v>
@@ -1413,24 +1418,24 @@
         <v>72</v>
       </c>
       <c r="H23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I23" s="1">
         <v>4</v>
       </c>
       <c r="J23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
         <v>79</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Added attract mode tunes
New intro music
Using IP's story tunes for attract cutscene
Timing still all busted
</commit_message>
<xml_diff>
--- a/Notes/music.xlsx
+++ b/Notes/music.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kconnell\OneDrive\BEEB\Repos\pop-beeb\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="444" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{91BD5E2F-22B9-41B3-92FF-9F919304701F}"/>
+  <xr:revisionPtr revIDLastSave="480" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{59C8BA76-2DB4-4E08-97C9-B0C5AC8F422E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3218" windowHeight="1605" xr2:uid="{19CB3A3B-005F-4A7A-B3B3-7B2FCB2886A0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="128">
   <si>
     <t>Game music</t>
   </si>
@@ -177,12 +177,6 @@
     <t>pop_music_potion</t>
   </si>
   <si>
-    <t>pop_music_title</t>
-  </si>
-  <si>
-    <t>pop_music_mirror</t>
-  </si>
-  <si>
     <t>pop_music_intro</t>
   </si>
   <si>
@@ -394,6 +388,33 @@
   </si>
   <si>
     <t>m-killguard-or-sword</t>
+  </si>
+  <si>
+    <t>intro_theme</t>
+  </si>
+  <si>
+    <t>story_1_absence</t>
+  </si>
+  <si>
+    <t>story_2_princess</t>
+  </si>
+  <si>
+    <t>story_3_Jaffar_enters</t>
+  </si>
+  <si>
+    <t>story_4_Jaffar_leaves</t>
+  </si>
+  <si>
+    <t>won</t>
+  </si>
+  <si>
+    <t>m-intro-wrongsignaturevgm</t>
+  </si>
+  <si>
+    <t>m-story2</t>
+  </si>
+  <si>
+    <t>m-story4</t>
   </si>
 </sst>
 </file>
@@ -443,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -456,6 +477,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864DF1D0-1AEF-4269-82FC-BFE1E4A43248}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -813,28 +840,28 @@
         <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
@@ -848,16 +875,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
         <v>44</v>
@@ -866,7 +893,7 @@
         <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
@@ -877,28 +904,28 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I4" s="1">
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -909,19 +936,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
         <v>45</v>
@@ -930,7 +957,7 @@
         <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
@@ -947,13 +974,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
         <v>46</v>
@@ -962,7 +989,7 @@
         <v>3</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
@@ -979,22 +1006,22 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" t="s">
         <v>110</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" t="s">
-        <v>112</v>
       </c>
       <c r="I7" s="1">
         <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
@@ -1005,28 +1032,28 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I8" s="1">
         <v>3</v>
       </c>
       <c r="J8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
@@ -1040,16 +1067,16 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
         <v>46</v>
@@ -1058,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
@@ -1072,18 +1099,17 @@
         <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H10" s="5"/>
+        <v>99</v>
+      </c>
       <c r="I10" s="1">
         <v>3</v>
       </c>
@@ -1099,25 +1125,25 @@
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I11" s="1">
         <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
@@ -1134,22 +1160,22 @@
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>117</v>
+        <v>73</v>
+      </c>
+      <c r="H12" t="s">
+        <v>115</v>
       </c>
       <c r="I12" s="1">
         <v>3</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
@@ -1163,25 +1189,25 @@
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I13" s="1">
         <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
@@ -1198,13 +1224,13 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H14" t="s">
         <v>47</v>
@@ -1213,12 +1239,12 @@
         <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" s="4"/>
       <c r="D16" s="4"/>
@@ -1235,25 +1261,25 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I17" s="1">
         <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
@@ -1264,25 +1290,25 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I18" s="1">
         <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
@@ -1293,25 +1319,25 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I19" s="1">
         <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
@@ -1322,25 +1348,25 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I20" s="1">
         <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
@@ -1351,16 +1377,16 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>45</v>
@@ -1377,25 +1403,25 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I22" s="1">
         <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
@@ -1406,42 +1432,42 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I23" s="1">
         <v>4</v>
       </c>
       <c r="J23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -1462,11 +1488,17 @@
       <c r="B27" s="1">
         <v>1</v>
       </c>
+      <c r="G27" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="H27" t="s">
         <v>48</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
@@ -1476,6 +1508,9 @@
       <c r="B28" s="1">
         <v>2</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
@@ -1484,11 +1519,8 @@
       <c r="B29" s="1">
         <v>3</v>
       </c>
-      <c r="H29" t="s">
-        <v>49</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0</v>
+      <c r="G29" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
@@ -1498,11 +1530,11 @@
       <c r="B30" s="1">
         <v>4</v>
       </c>
-      <c r="H30" t="s">
-        <v>50</v>
+      <c r="G30" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="I30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
@@ -1512,62 +1544,98 @@
       <c r="B31" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G31" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="1">
         <v>7</v>
       </c>
-      <c r="H33" t="s">
-        <v>50</v>
+      <c r="G33" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="I33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G34" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>37</v>
       </c>
       <c r="B35" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G35" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G36" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G37" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>40</v>
       </c>
       <c r="B38" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G38" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="1">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
@@ -1578,15 +1646,21 @@
       <c r="G40" s="4"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G41" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I41" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Starting to get the attract sequence music & timing sorted
Still a way to go
</commit_message>
<xml_diff>
--- a/Notes/music.xlsx
+++ b/Notes/music.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kconnell\OneDrive\BEEB\Repos\pop-beeb\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="480" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{59C8BA76-2DB4-4E08-97C9-B0C5AC8F422E}"/>
+  <xr:revisionPtr revIDLastSave="527" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{0D4A13E6-152E-4DCE-9B35-141440348ED4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3218" windowHeight="1605" xr2:uid="{19CB3A3B-005F-4A7A-B3B3-7B2FCB2886A0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="142">
   <si>
     <t>Game music</t>
   </si>
@@ -415,6 +415,48 @@
   </si>
   <si>
     <t>m-story4</t>
+  </si>
+  <si>
+    <t>pop_music_princess</t>
+  </si>
+  <si>
+    <t>pop_music_leaves</t>
+  </si>
+  <si>
+    <t>pop_music_sumup</t>
+  </si>
+  <si>
+    <t>Broderbund presents appears after 0:02</t>
+  </si>
+  <si>
+    <t>A game by Jordan Mechner appears after 0:07</t>
+  </si>
+  <si>
+    <t>Title screen appears after 0:15</t>
+  </si>
+  <si>
+    <t>Sultan's absence screen</t>
+  </si>
+  <si>
+    <t>Princess standing towards window</t>
+  </si>
+  <si>
+    <t>Princess turns around</t>
+  </si>
+  <si>
+    <t>Jaffar enters</t>
+  </si>
+  <si>
+    <t>Hourglass appears after 0:13</t>
+  </si>
+  <si>
+    <t>As Jaffar turns around and walks off</t>
+  </si>
+  <si>
+    <t>Music continues from story_4_Jaffar_leaves</t>
+  </si>
+  <si>
+    <t>As sand starts to flow</t>
   </si>
 </sst>
 </file>
@@ -464,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,6 +524,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -800,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864DF1D0-1AEF-4269-82FC-BFE1E4A43248}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1385,7 +1431,7 @@
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="7" t="s">
         <v>72</v>
       </c>
       <c r="H21" s="5" t="s">
@@ -1488,6 +1534,9 @@
       <c r="B27" s="1">
         <v>1</v>
       </c>
+      <c r="C27" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="G27" s="1" t="s">
         <v>119</v>
       </c>
@@ -1508,6 +1557,9 @@
       <c r="B28" s="1">
         <v>2</v>
       </c>
+      <c r="C28" s="9" t="s">
+        <v>132</v>
+      </c>
       <c r="G28" s="1" t="s">
         <v>99</v>
       </c>
@@ -1519,6 +1571,9 @@
       <c r="B29" s="1">
         <v>3</v>
       </c>
+      <c r="C29" s="9" t="s">
+        <v>133</v>
+      </c>
       <c r="G29" s="1" t="s">
         <v>99</v>
       </c>
@@ -1530,7 +1585,10 @@
       <c r="B30" s="1">
         <v>4</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="C30" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>120</v>
       </c>
       <c r="I30" s="1">
@@ -1544,8 +1602,14 @@
       <c r="B31" s="1">
         <v>5</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>68</v>
+      <c r="C31" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="I31" s="1">
         <v>0</v>
@@ -1561,8 +1625,14 @@
       <c r="B33" s="1">
         <v>7</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="C33" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" s="10" t="s">
         <v>121</v>
+      </c>
+      <c r="H33" t="s">
+        <v>128</v>
       </c>
       <c r="I33" s="1">
         <v>1</v>
@@ -1578,6 +1648,9 @@
       <c r="B34" s="1">
         <v>8</v>
       </c>
+      <c r="C34" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>99</v>
       </c>
@@ -1589,7 +1662,10 @@
       <c r="B35" s="1">
         <v>9</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="C35" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G35" s="10" t="s">
         <v>122</v>
       </c>
       <c r="I35" s="1">
@@ -1603,6 +1679,9 @@
       <c r="B36" s="1">
         <v>10</v>
       </c>
+      <c r="C36" s="9" t="s">
+        <v>138</v>
+      </c>
       <c r="G36" s="1" t="s">
         <v>99</v>
       </c>
@@ -1614,8 +1693,20 @@
       <c r="B37" s="1">
         <v>11</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>99</v>
+      <c r="C37" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H37" t="s">
+        <v>129</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
@@ -1625,14 +1716,11 @@
       <c r="B38" s="1">
         <v>12</v>
       </c>
-      <c r="G38" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="I38" s="1">
-        <v>1</v>
-      </c>
-      <c r="J38" t="s">
-        <v>127</v>
+      <c r="C38" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Added door creak to Story cutscene
</commit_message>
<xml_diff>
--- a/Notes/music.xlsx
+++ b/Notes/music.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kconnell\OneDrive\BEEB\Repos\pop-beeb\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="543" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{FE510777-D4CE-46B0-A0E0-7C5D75F30762}"/>
+  <xr:revisionPtr revIDLastSave="553" documentId="8_{9EA25EF8-2917-46A4-9E10-046A40919C1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{12D7A7DC-F8B5-4FF4-AD4C-155A416FE9C5}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3218" windowHeight="1605" xr2:uid="{19CB3A3B-005F-4A7A-B3B3-7B2FCB2886A0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="150">
   <si>
     <t>Game music</t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>pop_music_enters</t>
+  </si>
+  <si>
+    <t>doorcreak</t>
+  </si>
+  <si>
+    <t>m-embrace</t>
   </si>
 </sst>
 </file>
@@ -524,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -541,11 +547,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -865,7 +872,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1466,14 +1473,15 @@
       <c r="E22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="H22" s="5"/>
       <c r="I22" s="1">
         <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
@@ -1569,7 +1577,7 @@
       <c r="B28" s="1">
         <v>1</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>130</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -1592,7 +1600,7 @@
       <c r="B29" s="1">
         <v>2</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>131</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -1606,7 +1614,7 @@
       <c r="B30" s="1">
         <v>3</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>132</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -1620,7 +1628,7 @@
       <c r="B31" s="1">
         <v>4</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>133</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -1640,17 +1648,17 @@
       <c r="B32" s="1">
         <v>5</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H32" s="10" t="s">
         <v>129</v>
       </c>
       <c r="I32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="s">
         <v>112</v>
@@ -1663,10 +1671,10 @@
       <c r="B34" s="1">
         <v>7</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="9" t="s">
         <v>120</v>
       </c>
       <c r="H34" t="s">
@@ -1686,11 +1694,15 @@
       <c r="B35" s="1">
         <v>8</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>135</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>98</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="J35" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
@@ -1700,10 +1712,10 @@
       <c r="B36" s="1">
         <v>9</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="9" t="s">
         <v>121</v>
       </c>
       <c r="H36" t="s">
@@ -1723,7 +1735,7 @@
       <c r="B37" s="1">
         <v>10</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="8" t="s">
         <v>137</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -1737,10 +1749,10 @@
       <c r="B38" s="1">
         <v>11</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="11" t="s">
         <v>122</v>
       </c>
       <c r="H38" t="s">
@@ -1760,7 +1772,7 @@
       <c r="B39" s="1">
         <v>12</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="8" t="s">
         <v>138</v>
       </c>
       <c r="G39" s="1" t="s">

</xml_diff>